<commit_message>
Fix Bugs and create few modules
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11219"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Neo\Desktop\Source Files\Java Source Files\XLSX2SQLite\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/veronicatjan/eclipse-workspace/XLS2SQLITE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{534D3B4C-C219-418D-B48A-17C1D9F1C877}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5BE9472-47B6-B04F-AE91-4AF9A7654AEE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9588" xr2:uid="{11DCE840-D37F-459E-A0D6-035C6BF79A8D}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23040" windowHeight="9580" xr2:uid="{11DCE840-D37F-459E-A0D6-035C6BF79A8D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,48 +25,76 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Stephen</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Math</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>English</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Java</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>Veronica Tjan</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>veronicatjan@hotmail.com</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>13250808969</t>
+  </si>
+  <si>
+    <t>Sarah Huang</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>sarahhuang@gmail.com</t>
+  </si>
+  <si>
+    <t>13235812152</t>
+  </si>
+  <si>
+    <t>Email</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -89,21 +117,31 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -119,7 +157,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -415,15 +453,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5637B839-453C-4E97-98A9-588BB93412B8}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
+    <col min="5" max="5" width="17.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -434,32 +477,56 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
-        <v>75</v>
-      </c>
-      <c r="C2" s="1">
-        <v>98.5</v>
-      </c>
-      <c r="D2" s="1">
-        <v>96</v>
-      </c>
-      <c r="E2" s="1">
-        <v>100</v>
-      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E9" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{6FED341E-E10F-2A4C-BA8C-70402CDFA17E}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{9DA9EAE9-50A5-1E4E-AD51-B27EA108C9F9}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>